<commit_message>
Cleaning up the detailed summary table.
</commit_message>
<xml_diff>
--- a/DetailedSummaryTable.xlsx
+++ b/DetailedSummaryTable.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="20">
   <si>
     <t>Turnout</t>
   </si>
@@ -52,9 +52,6 @@
   </si>
   <si>
     <t>Voting center relocations</t>
-  </si>
-  <si>
-    <t>Ballot Box Stuffing (Potential)</t>
   </si>
   <si>
     <t>Absolute votes</t>
@@ -281,10 +278,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -340,14 +343,20 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="15">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
@@ -384,8 +393,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="I17:K22" totalsRowShown="0">
-  <autoFilter ref="I17:K22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="I22:K27" totalsRowShown="0">
+  <autoFilter ref="I22:K27">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -696,10 +705,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:L22"/>
+  <dimension ref="A2:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -716,22 +725,22 @@
         <v>5</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="6" t="s">
-        <v>18</v>
-      </c>
       <c r="G2" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -801,7 +810,7 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" s="12">
         <f>B4-B3</f>
@@ -830,22 +839,22 @@
         <v>6</v>
       </c>
       <c r="B8" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="D8" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="E8" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="F8" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="15" t="s">
-        <v>18</v>
-      </c>
       <c r="G8" s="16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -942,22 +951,22 @@
         <v>0</v>
       </c>
       <c r="B14" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="24" t="s">
+      <c r="D14" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="24" t="s">
+      <c r="E14" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="24" t="s">
+      <c r="F14" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="F14" s="24" t="s">
-        <v>18</v>
-      </c>
       <c r="G14" s="25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -1024,19 +1033,10 @@
       </c>
       <c r="F17" s="27"/>
       <c r="G17" s="28"/>
-      <c r="I17" t="s">
-        <v>13</v>
-      </c>
-      <c r="J17" t="s">
-        <v>11</v>
-      </c>
-      <c r="K17" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="29" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18" s="30">
         <f>B16-B15</f>
@@ -1059,83 +1059,80 @@
         <f>C18-F18</f>
         <v>6.7333418908076259E-2</v>
       </c>
-      <c r="I18" t="s">
+    </row>
+    <row r="22" spans="1:12">
+      <c r="I22" t="s">
+        <v>12</v>
+      </c>
+      <c r="J22" t="s">
+        <v>10</v>
+      </c>
+      <c r="K22" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="I23" t="s">
         <v>7</v>
       </c>
-      <c r="J18" s="3">
+      <c r="J23" s="3">
         <f>D18</f>
         <v>711182</v>
       </c>
-      <c r="K18" s="1">
+      <c r="K23" s="1">
         <f>C12-F18</f>
         <v>6.7333418908076259E-2</v>
       </c>
-      <c r="L18" s="2">
-        <f>J18/K18</f>
+      <c r="L23" s="2">
+        <f>J23/K23</f>
         <v>10562095.487396939</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
-      <c r="I19" t="s">
+    <row r="24" spans="1:12">
+      <c r="I24" t="s">
         <v>9</v>
       </c>
-      <c r="J19" s="3">
+      <c r="J24" s="3">
         <f>D3-D4</f>
         <v>19495</v>
       </c>
-      <c r="K19" s="1">
+      <c r="K24" s="1">
         <f>G6</f>
         <v>1.9857064634907218E-3</v>
       </c>
-      <c r="L19" s="2">
-        <f>J19/K19</f>
+      <c r="L24" s="2">
+        <f>J24/K24</f>
         <v>9817664.5735086463</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
-      <c r="I20" t="s">
-        <v>10</v>
-      </c>
-      <c r="J20" s="3">
-        <v>4568</v>
-      </c>
-      <c r="K20" s="1">
-        <f>G6</f>
-        <v>1.9857064634907218E-3</v>
-      </c>
-      <c r="L20" s="2">
-        <f>J20/K20</f>
-        <v>2300440.7166856886</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12">
-      <c r="I21" t="s">
+    <row r="25" spans="1:12">
+      <c r="I25" t="s">
         <v>8</v>
       </c>
-      <c r="J21" s="3">
+      <c r="J25" s="3">
         <f>D9</f>
         <v>92210</v>
       </c>
-      <c r="K21" s="1">
+      <c r="K25" s="1">
         <f>G12</f>
         <v>9.1163064545298766E-3</v>
       </c>
-      <c r="L21" s="2">
-        <f>J21/K21</f>
+      <c r="L25" s="2">
+        <f>J25/K25</f>
         <v>10114842.064593058</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
-      <c r="I22" t="s">
+    <row r="26" spans="1:12">
+      <c r="I26" t="s">
         <v>1</v>
       </c>
-      <c r="J22" s="4">
-        <f>SUM(J18:J21)</f>
-        <v>827455</v>
-      </c>
-      <c r="K22" s="1">
-        <f>SUM(K18:K21)</f>
-        <v>8.0421138289587579E-2</v>
+      <c r="J26" s="4">
+        <f>SUM(J23:J25)</f>
+        <v>822887</v>
+      </c>
+      <c r="K26" s="1">
+        <f>SUM(K23:K25)</f>
+        <v>7.8435431826096857E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding analysis on MCM's primary vote share, and correcting the Detailed Summary Table.
</commit_message>
<xml_diff>
--- a/DetailedSummaryTable.xlsx
+++ b/DetailedSummaryTable.xlsx
@@ -697,7 +697,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -708,7 +708,7 @@
   <dimension ref="A2:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -869,15 +869,15 @@
         <v>0.46146544204898016</v>
       </c>
       <c r="D9" s="18">
-        <v>92210</v>
+        <v>92105</v>
       </c>
       <c r="E9" s="18">
         <f>B9+D9</f>
-        <v>5077040</v>
+        <v>5076935</v>
       </c>
       <c r="F9" s="18">
         <f>E9/E11</f>
-        <v>0.4660235952762451</v>
+        <v>0.46601844876563192</v>
       </c>
       <c r="G9" s="19"/>
     </row>
@@ -899,7 +899,7 @@
       </c>
       <c r="F10" s="18">
         <f>E10/E11</f>
-        <v>0.53397640472375496</v>
+        <v>0.53398155123436808</v>
       </c>
       <c r="G10" s="19"/>
     </row>
@@ -915,7 +915,7 @@
       <c r="D11" s="18"/>
       <c r="E11" s="18">
         <f>SUM(E9:E10)</f>
-        <v>10894384</v>
+        <v>10894279</v>
       </c>
       <c r="F11" s="18"/>
       <c r="G11" s="19"/>
@@ -934,16 +934,16 @@
       </c>
       <c r="D12" s="21">
         <f>D9-D10</f>
-        <v>92210</v>
+        <v>92105</v>
       </c>
       <c r="E12" s="21"/>
       <c r="F12" s="21">
         <f>F10-F9</f>
-        <v>6.7952809447509865E-2</v>
+        <v>6.7963102468736158E-2</v>
       </c>
       <c r="G12" s="22">
         <f>C12-F12</f>
-        <v>9.1163064545298766E-3</v>
+        <v>9.1060134333035836E-3</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="28">
@@ -1111,15 +1111,15 @@
       </c>
       <c r="J25" s="3">
         <f>D9</f>
-        <v>92210</v>
+        <v>92105</v>
       </c>
       <c r="K25" s="1">
         <f>G12</f>
-        <v>9.1163064545298766E-3</v>
+        <v>9.1060134333035836E-3</v>
       </c>
       <c r="L25" s="2">
         <f>J25/K25</f>
-        <v>10114842.064593058</v>
+        <v>10114744.577813026</v>
       </c>
     </row>
     <row r="26" spans="1:12">
@@ -1128,11 +1128,11 @@
       </c>
       <c r="J26" s="4">
         <f>SUM(J23:J25)</f>
-        <v>822887</v>
+        <v>822782</v>
       </c>
       <c r="K26" s="1">
         <f>SUM(K23:K25)</f>
-        <v>7.8435431826096857E-2</v>
+        <v>7.8425138804870564E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correcting summary table to reflect actual vote totals in our data (as opposed to CNE website). See README.
</commit_message>
<xml_diff>
--- a/DetailedSummaryTable.xlsx
+++ b/DetailedSummaryTable.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="27729"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\francisco.rodriguez\AppData\Local\Packages\Microsoft.MicrosoftEdge_8wekyb3d8bbwe\TempState\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24960" windowHeight="16740"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="171027"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -87,7 +92,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0%"/>
@@ -393,16 +398,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="I22:K27" totalsRowShown="0">
-  <autoFilter ref="I22:K27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="I22:K27" totalsRowShown="0">
+  <autoFilter ref="I22:K27" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" name="Effect"/>
-    <tableColumn id="2" name="Absolute votes"/>
-    <tableColumn id="3" name="Percentage of total votes" dataDxfId="0" dataCellStyle="Percent"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Effect"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Absolute votes"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Percentage of total votes" dataDxfId="0" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -697,30 +702,30 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="7" width="11.33203125" customWidth="1"/>
+    <col min="2" max="7" width="11.28515625" customWidth="1"/>
     <col min="9" max="9" width="30" customWidth="1"/>
-    <col min="10" max="11" width="26.33203125" customWidth="1"/>
-    <col min="12" max="12" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="26.28515625" customWidth="1"/>
+    <col min="12" max="12" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" ht="28">
+    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
@@ -743,82 +748,82 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="9">
-        <v>4984830</v>
+        <v>4978522</v>
       </c>
       <c r="C3" s="9">
         <f>B3/B5</f>
-        <v>0.46146544204898016</v>
+        <v>0.46176503187634749</v>
       </c>
       <c r="D3" s="9">
         <v>22766</v>
       </c>
       <c r="E3" s="9">
         <f>B3+D3</f>
-        <v>5007596</v>
+        <v>5001288</v>
       </c>
       <c r="F3" s="9">
         <f>E3/E5</f>
-        <v>0.46245829528072552</v>
+        <v>0.46275906214382512</v>
       </c>
       <c r="G3" s="10"/>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="9">
-        <v>5817344</v>
+        <v>5802983</v>
       </c>
       <c r="C4" s="9">
         <f>B4/B5</f>
-        <v>0.5385345579510199</v>
+        <v>0.53823496812365246</v>
       </c>
       <c r="D4" s="9">
         <v>3271</v>
       </c>
       <c r="E4" s="9">
         <f>B4+D4</f>
-        <v>5820615</v>
+        <v>5806254</v>
       </c>
       <c r="F4" s="9">
         <f>E4/E5</f>
-        <v>0.53754170471927454</v>
+        <v>0.53724093785617488</v>
       </c>
       <c r="G4" s="10"/>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="9">
         <f>SUM(B3:B4)</f>
-        <v>10802174</v>
+        <v>10781505</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
       <c r="E5" s="9">
         <f>SUM(E3:E4)</f>
-        <v>10828211</v>
+        <v>10807542</v>
       </c>
       <c r="F5" s="9"/>
       <c r="G5" s="10"/>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>18</v>
       </c>
       <c r="B6" s="12">
         <f>B4-B3</f>
-        <v>832514</v>
+        <v>824461</v>
       </c>
       <c r="C6" s="12">
         <f>C4-C3</f>
-        <v>7.7069115902039742E-2</v>
+        <v>7.646993624730497E-2</v>
       </c>
       <c r="D6" s="12">
         <f>D3-D4</f>
@@ -827,14 +832,14 @@
       <c r="E6" s="12"/>
       <c r="F6" s="12">
         <f>F4-F3</f>
-        <v>7.508340943854902E-2</v>
+        <v>7.4481875712349765E-2</v>
       </c>
       <c r="G6" s="13">
         <f>C6-F6</f>
-        <v>1.9857064634907218E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="28">
+        <v>1.988060534955205E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>6</v>
       </c>
@@ -857,80 +862,80 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
         <v>2</v>
       </c>
       <c r="B9" s="18">
-        <v>4984830</v>
+        <v>4978522</v>
       </c>
       <c r="C9" s="18">
         <f>B9/B11</f>
-        <v>0.46146544204898016</v>
+        <v>0.46176503187634749</v>
       </c>
       <c r="D9" s="18">
         <v>92105</v>
       </c>
       <c r="E9" s="18">
         <f>B9+D9</f>
-        <v>5076935</v>
+        <v>5070627</v>
       </c>
       <c r="F9" s="18">
         <f>E9/E11</f>
-        <v>0.46601844876563192</v>
+        <v>0.466324155455272</v>
       </c>
       <c r="G9" s="19"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
         <v>3</v>
       </c>
       <c r="B10" s="18">
-        <v>5817344</v>
+        <v>5802983</v>
       </c>
       <c r="C10" s="18">
         <f>B10/B11</f>
-        <v>0.5385345579510199</v>
+        <v>0.53823496812365246</v>
       </c>
       <c r="D10" s="18"/>
       <c r="E10" s="18">
         <f>B10+D10</f>
-        <v>5817344</v>
+        <v>5802983</v>
       </c>
       <c r="F10" s="18">
         <f>E10/E11</f>
-        <v>0.53398155123436808</v>
+        <v>0.53367584454472805</v>
       </c>
       <c r="G10" s="19"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
         <v>1</v>
       </c>
       <c r="B11" s="18">
         <f>SUM(B9:B10)</f>
-        <v>10802174</v>
+        <v>10781505</v>
       </c>
       <c r="C11" s="18"/>
       <c r="D11" s="18"/>
       <c r="E11" s="18">
         <f>SUM(E9:E10)</f>
-        <v>10894279</v>
+        <v>10873610</v>
       </c>
       <c r="F11" s="18"/>
       <c r="G11" s="19"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
         <v>4</v>
       </c>
       <c r="B12" s="21">
         <f>B10-B9</f>
-        <v>832514</v>
+        <v>824461</v>
       </c>
       <c r="C12" s="21">
         <f>C10-C9</f>
-        <v>7.7069115902039742E-2</v>
+        <v>7.646993624730497E-2</v>
       </c>
       <c r="D12" s="21">
         <f>D9-D10</f>
@@ -939,14 +944,14 @@
       <c r="E12" s="21"/>
       <c r="F12" s="21">
         <f>F10-F9</f>
-        <v>6.7963102468736158E-2</v>
+        <v>6.7351689089456046E-2</v>
       </c>
       <c r="G12" s="22">
         <f>C12-F12</f>
-        <v>9.1060134333035836E-3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="28">
+        <v>9.1182471578489244E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="23" t="s">
         <v>0</v>
       </c>
@@ -969,20 +974,20 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="26" t="s">
         <v>2</v>
       </c>
       <c r="B15" s="27">
-        <v>4984830</v>
+        <v>4978522</v>
       </c>
       <c r="C15" s="27">
         <f>B15/B17</f>
-        <v>0.46146544204898016</v>
+        <v>0.46176503187634749</v>
       </c>
       <c r="D15" s="27">
         <f>E15-B15</f>
-        <v>1185799</v>
+        <v>1192107</v>
       </c>
       <c r="E15" s="27">
         <v>6170629</v>
@@ -993,20 +998,20 @@
       </c>
       <c r="G15" s="28"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="26" t="s">
         <v>3</v>
       </c>
       <c r="B16" s="27">
-        <v>5817344</v>
+        <v>5802983</v>
       </c>
       <c r="C16" s="27">
         <f>B16/B17</f>
-        <v>0.5385345579510199</v>
+        <v>0.53823496812365246</v>
       </c>
       <c r="D16" s="27">
         <f>E16-B16</f>
-        <v>474617</v>
+        <v>488978</v>
       </c>
       <c r="E16" s="27">
         <v>6291961</v>
@@ -1017,13 +1022,13 @@
       </c>
       <c r="G16" s="28"/>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="26" t="s">
         <v>1</v>
       </c>
       <c r="B17" s="27">
         <f>SUM(B15:B16)</f>
-        <v>10802174</v>
+        <v>10781505</v>
       </c>
       <c r="C17" s="27"/>
       <c r="D17" s="27"/>
@@ -1034,21 +1039,21 @@
       <c r="F17" s="27"/>
       <c r="G17" s="28"/>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="29" t="s">
         <v>18</v>
       </c>
       <c r="B18" s="30">
         <f>B16-B15</f>
-        <v>832514</v>
+        <v>824461</v>
       </c>
       <c r="C18" s="30">
         <f>C16-C15</f>
-        <v>7.7069115902039742E-2</v>
+        <v>7.646993624730497E-2</v>
       </c>
       <c r="D18" s="30">
         <f>D15-D16</f>
-        <v>711182</v>
+        <v>703129</v>
       </c>
       <c r="E18" s="30"/>
       <c r="F18" s="30">
@@ -1057,10 +1062,10 @@
       </c>
       <c r="G18" s="31">
         <f>C18-F18</f>
-        <v>6.7333418908076259E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12">
+        <v>6.6734239253341487E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I22" t="s">
         <v>12</v>
       </c>
@@ -1071,24 +1076,24 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I23" t="s">
         <v>7</v>
       </c>
       <c r="J23" s="3">
         <f>D18</f>
-        <v>711182</v>
+        <v>703129</v>
       </c>
       <c r="K23" s="1">
         <f>C12-F18</f>
-        <v>6.7333418908076259E-2</v>
+        <v>6.6734239253341487E-2</v>
       </c>
       <c r="L23" s="2">
         <f>J23/K23</f>
-        <v>10562095.487396939</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12">
+        <v>10536255.569359671</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I24" t="s">
         <v>9</v>
       </c>
@@ -1098,14 +1103,14 @@
       </c>
       <c r="K24" s="1">
         <f>G6</f>
-        <v>1.9857064634907218E-3</v>
+        <v>1.988060534955205E-3</v>
       </c>
       <c r="L24" s="2">
         <f>J24/K24</f>
-        <v>9817664.5735086463</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12">
+        <v>9806039.4325162042</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I25" t="s">
         <v>8</v>
       </c>
@@ -1115,24 +1120,24 @@
       </c>
       <c r="K25" s="1">
         <f>G12</f>
-        <v>9.1060134333035836E-3</v>
+        <v>9.1182471578489244E-3</v>
       </c>
       <c r="L25" s="2">
         <f>J25/K25</f>
-        <v>10114744.577813026</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12">
+        <v>10101173.877560081</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I26" t="s">
         <v>1</v>
       </c>
       <c r="J26" s="4">
         <f>SUM(J23:J25)</f>
-        <v>822782</v>
+        <v>814729</v>
       </c>
       <c r="K26" s="1">
         <f>SUM(K23:K25)</f>
-        <v>7.8425138804870564E-2</v>
+        <v>7.7840546946145617E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>